<commit_message>
cleaned up plots with viridis
</commit_message>
<xml_diff>
--- a/ccb_proj_mgt.xlsx
+++ b/ccb_proj_mgt.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112671/Documents/tmp/ccb_project_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F00745D4-6D49-9B4D-B08C-C4D9AC59503D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0ECB7EC-19D8-A14D-81CE-7B3E9E747546}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{26031F6B-AA17-7943-AEA2-E25B1637DE85}"/>
   </bookViews>
@@ -96,9 +96,6 @@
     <t>Installation of MAGeCK-VISPR</t>
   </si>
   <si>
-    <t>CRISPR-Cas9</t>
-  </si>
-  <si>
     <t>Mazzone</t>
   </si>
   <si>
@@ -195,9 +192,6 @@
     <t>There were 2 versions of this analysis</t>
   </si>
   <si>
-    <t>Differential Expression + GSEA</t>
-  </si>
-  <si>
     <t>There were 4 versions of this analysis</t>
   </si>
   <si>
@@ -328,6 +322,12 @@
   </si>
   <si>
     <t>Extension of previous RNAseq analysis, this time with new samples</t>
+  </si>
+  <si>
+    <t>DE + GSEA</t>
+  </si>
+  <si>
+    <t>CRISPR screen</t>
   </si>
 </sst>
 </file>
@@ -692,14 +692,14 @@
   <dimension ref="A1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="55.5" customWidth="1"/>
     <col min="2" max="2" width="15.5" customWidth="1"/>
-    <col min="3" max="3" width="27.5" customWidth="1"/>
+    <col min="3" max="3" width="17.5" customWidth="1"/>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
     <col min="6" max="6" width="12.5" customWidth="1"/>
@@ -709,13 +709,13 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
@@ -744,7 +744,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>56</v>
+        <v>99</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -756,13 +756,13 @@
         <v>44061</v>
       </c>
       <c r="G2">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="H2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -773,7 +773,7 @@
         <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D3" t="s">
         <v>13</v>
@@ -802,7 +802,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -820,18 +820,18 @@
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -849,7 +849,7 @@
         <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -857,16 +857,16 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" t="s">
+        <v>65</v>
+      </c>
+      <c r="E6" t="s">
         <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" t="s">
-        <v>67</v>
-      </c>
-      <c r="E6" t="s">
-        <v>24</v>
       </c>
       <c r="F6" s="1">
         <v>44074</v>
@@ -878,21 +878,21 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7" t="s">
         <v>25</v>
-      </c>
-      <c r="B7" t="s">
-        <v>42</v>
-      </c>
-      <c r="C7" t="s">
-        <v>51</v>
-      </c>
-      <c r="D7" t="s">
-        <v>26</v>
       </c>
       <c r="E7" t="s">
         <v>18</v>
@@ -907,24 +907,24 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
         <v>27</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
         <v>28</v>
       </c>
-      <c r="C8" t="s">
-        <v>56</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>29</v>
-      </c>
-      <c r="E8" t="s">
-        <v>30</v>
       </c>
       <c r="F8" s="1">
         <v>44080</v>
@@ -936,24 +936,24 @@
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-      <c r="B9" t="s">
-        <v>28</v>
-      </c>
       <c r="C9" t="s">
+        <v>99</v>
+      </c>
+      <c r="D9" t="s">
         <v>56</v>
       </c>
-      <c r="D9" t="s">
-        <v>58</v>
-      </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F9" s="1">
         <v>44080</v>
@@ -965,24 +965,24 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" t="s">
         <v>31</v>
       </c>
-      <c r="B10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>32</v>
-      </c>
       <c r="E10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F10" s="1">
         <v>44080</v>
@@ -994,24 +994,24 @@
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F11" s="1">
         <v>44090</v>
@@ -1023,24 +1023,24 @@
         <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F12" s="1">
         <v>44081</v>
@@ -1052,24 +1052,24 @@
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F13" s="1">
         <v>44102</v>
@@ -1081,7 +1081,7 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1089,16 +1089,16 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
         <v>29</v>
-      </c>
-      <c r="E14" t="s">
-        <v>30</v>
       </c>
       <c r="F14" s="1">
         <v>44103</v>
@@ -1110,24 +1110,24 @@
         <v>10</v>
       </c>
       <c r="I14" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" t="s">
+        <v>36</v>
+      </c>
+      <c r="E15" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>39</v>
       </c>
       <c r="F15" s="1">
         <v>44103</v>
@@ -1139,24 +1139,24 @@
         <v>19</v>
       </c>
       <c r="I15" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" t="s">
-        <v>23</v>
-      </c>
-      <c r="C16" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F16" s="1">
         <v>44118</v>
@@ -1168,24 +1168,24 @@
         <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D17" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F17" s="1">
         <v>44139</v>
@@ -1194,27 +1194,27 @@
         <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C18" t="s">
+        <v>99</v>
+      </c>
+      <c r="D18" t="s">
         <v>56</v>
       </c>
-      <c r="D18" t="s">
-        <v>58</v>
-      </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F18" s="1">
         <v>44155</v>
@@ -1226,53 +1226,53 @@
         <v>19</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C19" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" t="s">
         <v>62</v>
       </c>
-      <c r="B19" t="s">
+      <c r="E19" t="s">
         <v>63</v>
-      </c>
-      <c r="C19" t="s">
-        <v>35</v>
-      </c>
-      <c r="D19" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" t="s">
-        <v>65</v>
       </c>
       <c r="F19" s="1">
         <v>44186</v>
       </c>
       <c r="G19">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="H19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I19" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="B20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F20" s="1">
         <v>44213</v>
@@ -1284,24 +1284,24 @@
         <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21" t="s">
         <v>27</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
+        <v>99</v>
+      </c>
+      <c r="D21" t="s">
         <v>28</v>
       </c>
-      <c r="C21" t="s">
-        <v>56</v>
-      </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>29</v>
-      </c>
-      <c r="E21" t="s">
-        <v>30</v>
       </c>
       <c r="F21" s="1">
         <v>44217</v>
@@ -1313,53 +1313,53 @@
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B22" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" t="s">
+        <v>77</v>
+      </c>
+      <c r="D22" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" t="s">
         <v>23</v>
-      </c>
-      <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="D22" t="s">
-        <v>70</v>
-      </c>
-      <c r="E22" t="s">
-        <v>24</v>
       </c>
       <c r="F22" s="1">
         <v>44217</v>
       </c>
       <c r="G22">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I22" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D23" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F23" s="1">
         <v>44217</v>
@@ -1368,27 +1368,27 @@
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I23" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E24" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F24" s="1">
         <v>44222</v>
@@ -1397,27 +1397,27 @@
         <v>10</v>
       </c>
       <c r="H24" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E25" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="F25" s="1">
         <v>44229</v>
@@ -1426,24 +1426,24 @@
         <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="B26" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F26" s="1">
         <v>44237</v>
@@ -1452,36 +1452,36 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I26" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B27" t="s">
+        <v>77</v>
+      </c>
+      <c r="C27" t="s">
+        <v>77</v>
+      </c>
+      <c r="D27" t="s">
         <v>79</v>
       </c>
-      <c r="C27" t="s">
-        <v>79</v>
-      </c>
-      <c r="D27" t="s">
-        <v>81</v>
-      </c>
       <c r="E27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F27" s="1">
         <v>44238</v>
       </c>
       <c r="G27">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H27" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
22 march changes, fixed plots
</commit_message>
<xml_diff>
--- a/ccb_proj_mgt.xlsx
+++ b/ccb_proj_mgt.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/u0112671/Documents/tmp/ccb_project_management/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{467600AD-E1BA-CD49-A6B7-74480640C3DE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A13F9CB-8414-B441-A68C-AEA11DF7885F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{26031F6B-AA17-7943-AEA2-E25B1637DE85}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="114">
   <si>
     <t>project_type</t>
   </si>
@@ -150,9 +150,6 @@
     <t>Analysis of CNV data</t>
   </si>
   <si>
-    <t>biostatistics</t>
-  </si>
-  <si>
     <t>SNP Calling Pipeline for Single Cell Data</t>
   </si>
   <si>
@@ -189,12 +186,6 @@
     <t>Tommaso Scolaro</t>
   </si>
   <si>
-    <t>There were 2 versions of this analysis</t>
-  </si>
-  <si>
-    <t>There were 4 versions of this analysis</t>
-  </si>
-  <si>
     <t>Lindsay Broadfield</t>
   </si>
   <si>
@@ -252,9 +243,6 @@
     <t>WES Copy Number Pipeline</t>
   </si>
   <si>
-    <t>WES</t>
-  </si>
-  <si>
     <t>Epigenetics</t>
   </si>
   <si>
@@ -343,6 +331,42 @@
   </si>
   <si>
     <t>Benchmarking of EIF2AK3/PERK in Single Cell data</t>
+  </si>
+  <si>
+    <t>Benchmarking Publically Available Methylation Datasets</t>
+  </si>
+  <si>
+    <t>Ewout Landeloos</t>
+  </si>
+  <si>
+    <t>There were 4 versions of this analysis (i.e. different models)</t>
+  </si>
+  <si>
+    <t>There were 2 versions of this analysis (i.e. different models)</t>
+  </si>
+  <si>
+    <t>Ewout wants to test different methylation datasets and compare the results with his data</t>
+  </si>
+  <si>
+    <t>Benchmarking PERK in T-cells in two different datasets</t>
+  </si>
+  <si>
+    <t>Qun is benchmarking Single Cell Data and needed help with a script to extract the necessary files</t>
+  </si>
+  <si>
+    <t>Calra requested help in interpreting gene regulatory information with respect to her gene of interest, TRAIL</t>
+  </si>
+  <si>
+    <t>Benchmarking in 1 dataset</t>
+  </si>
+  <si>
+    <t>WES CN</t>
+  </si>
+  <si>
+    <t>Regulatory Analysis</t>
+  </si>
+  <si>
+    <t>Biostatistics</t>
   </si>
 </sst>
 </file>
@@ -704,10 +728,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7837E5B2-4544-3646-A14E-E013871A588B}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -724,7 +748,7 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
@@ -759,7 +783,7 @@
         <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -774,10 +798,10 @@
         <v>200</v>
       </c>
       <c r="H2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I2" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -817,7 +841,7 @@
         <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -835,18 +859,18 @@
         <v>19</v>
       </c>
       <c r="I4" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="B5" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D5" t="s">
         <v>20</v>
@@ -864,7 +888,7 @@
         <v>19</v>
       </c>
       <c r="I5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -872,13 +896,13 @@
         <v>22</v>
       </c>
       <c r="B6" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
         <v>34</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
         <v>23</v>
@@ -893,7 +917,7 @@
         <v>19</v>
       </c>
       <c r="I6" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -901,10 +925,10 @@
         <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="D7" t="s">
         <v>25</v>
@@ -922,7 +946,7 @@
         <v>19</v>
       </c>
       <c r="I7" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -933,7 +957,7 @@
         <v>27</v>
       </c>
       <c r="C8" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D8" t="s">
         <v>28</v>
@@ -951,7 +975,7 @@
         <v>19</v>
       </c>
       <c r="I8" t="s">
-        <v>54</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -962,10 +986,10 @@
         <v>27</v>
       </c>
       <c r="C9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D9" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E9" t="s">
         <v>29</v>
@@ -980,7 +1004,7 @@
         <v>19</v>
       </c>
       <c r="I9" t="s">
-        <v>55</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1009,21 +1033,21 @@
         <v>19</v>
       </c>
       <c r="I10" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B11" t="s">
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D11" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E11" t="s">
         <v>23</v>
@@ -1038,12 +1062,12 @@
         <v>19</v>
       </c>
       <c r="I11" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
         <v>8</v>
@@ -1052,7 +1076,7 @@
         <v>34</v>
       </c>
       <c r="D12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E12" t="s">
         <v>38</v>
@@ -1067,21 +1091,21 @@
         <v>19</v>
       </c>
       <c r="I12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B13" t="s">
         <v>8</v>
       </c>
       <c r="C13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D13" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E13" t="s">
         <v>23</v>
@@ -1096,7 +1120,7 @@
         <v>19</v>
       </c>
       <c r="I13" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1104,10 +1128,10 @@
         <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="C14" t="s">
-        <v>41</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
         <v>28</v>
@@ -1159,16 +1183,16 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C16" t="s">
         <v>34</v>
       </c>
       <c r="D16" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
         <v>29</v>
@@ -1183,21 +1207,21 @@
         <v>19</v>
       </c>
       <c r="I16" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
       <c r="C17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E17" t="s">
         <v>23</v>
@@ -1209,24 +1233,24 @@
         <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I17" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="B18" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D18" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E18" t="s">
         <v>29</v>
@@ -1241,24 +1265,24 @@
         <v>19</v>
       </c>
       <c r="I18" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="B19" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C19" t="s">
         <v>34</v>
       </c>
       <c r="D19" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F19" s="1">
         <v>44186</v>
@@ -1267,24 +1291,24 @@
         <v>18</v>
       </c>
       <c r="H19" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I19" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="B20" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="E20" t="s">
         <v>29</v>
@@ -1299,7 +1323,7 @@
         <v>19</v>
       </c>
       <c r="I20" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
@@ -1310,7 +1334,7 @@
         <v>27</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="D21" t="s">
         <v>28</v>
@@ -1328,21 +1352,21 @@
         <v>19</v>
       </c>
       <c r="I21" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>48</v>
       </c>
       <c r="D22" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
         <v>23</v>
@@ -1354,24 +1378,24 @@
         <v>25</v>
       </c>
       <c r="H22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I22" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D23" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E23" t="s">
         <v>23</v>
@@ -1383,24 +1407,24 @@
         <v>25</v>
       </c>
       <c r="H23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I23" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
         <v>8</v>
       </c>
       <c r="C24" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D24" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E24" t="s">
         <v>23</v>
@@ -1412,27 +1436,27 @@
         <v>22</v>
       </c>
       <c r="H24" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I24" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B25" t="s">
         <v>8</v>
       </c>
       <c r="C25" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D25" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="E25" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F25" s="1">
         <v>44229</v>
@@ -1441,21 +1465,24 @@
         <v>5</v>
       </c>
       <c r="H25" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="I25" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
         <v>34</v>
       </c>
       <c r="D26" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E26" t="s">
         <v>38</v>
@@ -1467,24 +1494,24 @@
         <v>1</v>
       </c>
       <c r="H26" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I26" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="B27" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>112</v>
       </c>
       <c r="D27" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E27" t="s">
         <v>23</v>
@@ -1496,12 +1523,15 @@
         <v>4</v>
       </c>
       <c r="H27" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="I27" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
         <v>8</v>
@@ -1510,7 +1540,7 @@
         <v>34</v>
       </c>
       <c r="D28" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E28" t="s">
         <v>14</v>
@@ -1524,19 +1554,22 @@
       <c r="H28" t="s">
         <v>19</v>
       </c>
+      <c r="I28" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B29" t="s">
         <v>8</v>
       </c>
       <c r="C29" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D29" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E29" t="s">
         <v>23</v>
@@ -1548,24 +1581,27 @@
         <v>5</v>
       </c>
       <c r="H29" t="s">
-        <v>52</v>
+        <v>19</v>
+      </c>
+      <c r="I29" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="B30" t="s">
         <v>8</v>
       </c>
       <c r="C30" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D30" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="E30" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F30" s="1">
         <v>44272</v>
@@ -1574,7 +1610,39 @@
         <v>8</v>
       </c>
       <c r="H30" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="I30" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>102</v>
+      </c>
+      <c r="B31" t="s">
+        <v>72</v>
+      </c>
+      <c r="C31" t="s">
+        <v>48</v>
+      </c>
+      <c r="D31" t="s">
+        <v>103</v>
+      </c>
+      <c r="E31" t="s">
+        <v>38</v>
+      </c>
+      <c r="F31" s="1">
+        <v>44277</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>51</v>
+      </c>
+      <c r="I31" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>